<commit_message>
Doc n class diagram in shared call
</commit_message>
<xml_diff>
--- a/completezza funzionale_backend.xlsx
+++ b/completezza funzionale_backend.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salvc\Desktop\Ratatouille23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBBAACE-9A61-49DE-964E-AE6FB6EFC454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7965F4DD-E396-4BF1-B11B-7E56A2D4B63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,18 +379,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -400,38 +395,6 @@
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Verdana"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -586,6 +549,38 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -600,7 +595,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4308D9E-9884-418A-9C23-B668F99BD116}" name="Tabella1" displayName="Tabella1" ref="A1:J19" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D4308D9E-9884-418A-9C23-B668F99BD116}" name="Tabella1" displayName="Tabella1" ref="A1:J19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:J19" xr:uid="{D4308D9E-9884-418A-9C23-B668F99BD116}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -614,16 +609,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{C9340832-7974-41A1-B8C8-53D8FD0599FD}" name="STEP" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{D418CEA3-FC0B-4380-AF13-8EB0BF6988B7}" name="Funzionalità #1" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{107A1F97-5194-4511-985B-11496ED9839C}" name="Funzionalità #2" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{C9173966-C68F-4AA6-9412-7A628456FC95}" name="Funzionalità #3" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{9F10B02B-5572-4A1B-B35F-135C511B66C6}" name="Funzionalità #4" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{271919E5-A037-41C6-86DD-FD147727025B}" name="Funzionalità #5" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{80812BDE-50C9-4FFD-8383-5439544E703A}" name="Funzionalità #6" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{14034861-9F72-4D5C-ABFE-432A5BD72B66}" name="Funzionalità #7" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{31202016-B786-4A9A-9EC5-F091FC128363}" name="Funzionalità #8" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{3B9BBA01-1BDB-4823-85F6-2CCEB684AF04}" name="ALTRI" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C9340832-7974-41A1-B8C8-53D8FD0599FD}" name="STEP" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{D418CEA3-FC0B-4380-AF13-8EB0BF6988B7}" name="Funzionalità #1" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{107A1F97-5194-4511-985B-11496ED9839C}" name="Funzionalità #2" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C9173966-C68F-4AA6-9412-7A628456FC95}" name="Funzionalità #3" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{9F10B02B-5572-4A1B-B35F-135C511B66C6}" name="Funzionalità #4" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{271919E5-A037-41C6-86DD-FD147727025B}" name="Funzionalità #5" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{80812BDE-50C9-4FFD-8383-5439544E703A}" name="Funzionalità #6" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{14034861-9F72-4D5C-ABFE-432A5BD72B66}" name="Funzionalità #7" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{31202016-B786-4A9A-9EC5-F091FC128363}" name="Funzionalità #8" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{3B9BBA01-1BDB-4823-85F6-2CCEB684AF04}" name="ALTRI" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -895,7 +890,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,67 +902,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>48</v>
       </c>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -994,15 +989,15 @@
       <c r="I3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1020,25 +1015,25 @@
       <c r="G4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>78</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1050,7 +1045,7 @@
       <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>79</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -1059,14 +1054,14 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1078,19 +1073,19 @@
       <c r="G6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1107,18 +1102,18 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1129,21 +1124,21 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>62</v>
       </c>
       <c r="H9" s="1"/>
@@ -1151,17 +1146,17 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>63</v>
       </c>
       <c r="H10" s="1"/>
@@ -1169,17 +1164,17 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>64</v>
       </c>
       <c r="H11" s="1"/>
@@ -1187,17 +1182,17 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H12" s="1"/>
@@ -1205,104 +1200,104 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="4" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="4" t="s">
+      <c r="F13" s="1"/>
+      <c r="G13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="4" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="4" t="s">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="4" t="s">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>